<commit_message>
Mise à jour des fichiers vers nouvelle version du  schéma
- Ajout de l'attribut Name
- created_date et last_modified_date : modification vers un datetime
</commit_message>
<xml_diff>
--- a/Schema_stationnements_velos_gabarit.xlsx
+++ b/Schema_stationnements_velos_gabarit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eliseho-pun-cheung/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valja\Downloads\standard-stationnements-velos-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADE0ED6-37CF-D34E-8D60-AF63E0709E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E327A64-BB83-4F16-8F0F-61ED1832EFC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1000" windowWidth="27240" windowHeight="15520" xr2:uid="{4EB78F95-14FF-4443-8F92-35C7A833E6FB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{4EB78F95-14FF-4443-8F92-35C7A833E6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="gabarit" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>repair_equipment</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -486,113 +489,114 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15403F86-3314-1E4A-91E9-5779C8A9E1C5}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Y2:Z2"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="26" width="18.83203125" customWidth="1"/>
-    <col min="27" max="27" width="25.1640625" customWidth="1"/>
-    <col min="28" max="29" width="18.83203125" customWidth="1"/>
+    <col min="1" max="27" width="18.796875" customWidth="1"/>
+    <col min="28" max="28" width="25.19921875" customWidth="1"/>
+    <col min="29" max="30" width="18.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Y1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -607,18 +611,19 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
-      <c r="Y2" s="2"/>
+      <c r="Y2" s="3"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="3"/>
+      <c r="AA2" s="2"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F2" xr:uid="{6F2E3C23-CE3D-1D45-82F9-1F03F472AFAA}">
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{6F2E3C23-CE3D-1D45-82F9-1F03F472AFAA}">
       <formula1>99999</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{C5965CBC-6D3A-B44C-BC8A-92AC3AE54BE0}">
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{C5965CBC-6D3A-B44C-BC8A-92AC3AE54BE0}">
       <formula1>99999999999999</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>